<commit_message>
Threading for halls part
</commit_message>
<xml_diff>
--- a/observer_output.xlsx
+++ b/observer_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16807" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16809" uniqueCount="392">
   <si>
     <t>الاسم</t>
   </si>
@@ -1977,6 +1977,9 @@
       <c r="H5" t="s">
         <v>391</v>
       </c>
+      <c r="I5" t="s">
+        <v>388</v>
+      </c>
       <c r="J5" t="s">
         <v>391</v>
       </c>
@@ -2033,6 +2036,9 @@
       </c>
       <c r="AB5" t="s">
         <v>391</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>388</v>
       </c>
       <c r="AD5" t="s">
         <v>391</v>

</xml_diff>